<commit_message>
psa farm history survey version 1.2
Changed question #43 from an integer to a text note. Regarding economic data, how much does it cost to apply herbicide?
</commit_message>
<xml_diff>
--- a/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
+++ b/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
@@ -17,12 +17,11 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="453">
   <si>
     <t>type</t>
   </si>
@@ -765,21 +764,12 @@
     <t>note_end</t>
   </si>
   <si>
-    <t>Thank you for completing the Survey. Swipe to the next screen for a Timeline to share with your grower. Continue swiping until you reach the end to Submit.</t>
-  </si>
-  <si>
     <t>note_to_farmer</t>
   </si>
   <si>
-    <t>TIMELINE -- a technician will be in contact this spring. Cover Crop biomass is collected in the spring at the time it is terminated.  For our safety it is nice to harvest biomass right before burndown. Please notify the technician when you think you will terminate, and we can harvest +/- 3 to 4 days around that time. We can also return following herbicide application, when safe to do so. We will return when the crop is planted.  When do you think that will be? How long after terminating the cover crop? It is important to record those dates. We will install moisture sensors in between the crop rows after it has emerged.  Please do all of your fertilizer applications, and other management operations the same as you always would in that field. Our equipment is designed to be sprayed over.  We will raise a solar panel after the crop has closed canopy. We will come take yield data by hand in a 10 foot section around the soil moisture sensors before you harvest with your combine. Please notify us when you will: terminate your cover crop, after crop planting, and before harvest.  Thank you.</t>
-  </si>
-  <si>
     <t>note_to_tech</t>
   </si>
   <si>
-    <t>Technician: If there are questions that you were unable to complete at this time, you may save the survey to your device to retrieve later by clicking the arrow with the dot, selecting 'Go to End', naming the form by the farm name,  and select "Save Form and Exit". Forms can be retrieved in your "Saved Forms"</t>
-  </si>
-  <si>
     <t>Are there any questions, comments, or concerns you want to record here?</t>
   </si>
   <si>
@@ -1362,9 +1352,6 @@
     <t>psa_farm_history_survey</t>
   </si>
   <si>
-    <t>v1.1</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -1378,6 +1365,21 @@
   </si>
   <si>
     <t>media::image</t>
+  </si>
+  <si>
+    <t>communicate.jpg</t>
+  </si>
+  <si>
+    <t>Thank you. Communicate with your grower</t>
+  </si>
+  <si>
+    <t>To SAVE: If there are questions that you were unable to complete at this time, you may save the survey to your device to retrieve later by clicking the arrow with the dot, selecting 'Go to End', naming the form by the farm name,  and select "Save Form and Exit". Forms can be retrieved in your "Saved Forms"</t>
+  </si>
+  <si>
+    <t>Thank you for completing the Survey. The next screen has a timeline to share with your grower. Continue swiping until you reach the end to Submit.</t>
+  </si>
+  <si>
+    <t>v1.2</t>
   </si>
 </sst>
 </file>
@@ -1721,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1761,10 +1763,10 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="K1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1822,7 +1824,7 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1839,7 +1841,7 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -3078,10 +3080,10 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B91" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C91" t="s">
         <v>225</v>
@@ -3169,7 +3171,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>173</v>
       </c>
@@ -3177,13 +3179,13 @@
         <v>240</v>
       </c>
       <c r="C97" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>45</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>17</v>
       </c>
@@ -3211,12 +3213,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>17</v>
       </c>
@@ -3224,49 +3226,52 @@
         <v>246</v>
       </c>
       <c r="C101" t="s">
-        <v>247</v>
+        <v>451</v>
       </c>
       <c r="E101" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C102" t="s">
-        <v>249</v>
+        <v>449</v>
       </c>
       <c r="E102" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K102" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C103" t="s">
-        <v>251</v>
+        <v>450</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>45</v>
       </c>
       <c r="B104" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C104" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E104" t="s">
         <v>15</v>
@@ -3287,7 +3292,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3298,1091 +3303,1091 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" t="s">
         <v>254</v>
       </c>
-      <c r="B3" t="s">
-        <v>257</v>
-      </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" t="s">
         <v>259</v>
       </c>
-      <c r="B5" t="s">
-        <v>262</v>
-      </c>
       <c r="C5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B6" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B7" t="s">
         <v>264</v>
       </c>
-      <c r="B7" t="s">
-        <v>267</v>
-      </c>
       <c r="C7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C12" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B13" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C13" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C14" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B15" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B16" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C16" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B17" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C17" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B18" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C18" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B19" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C19" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B20" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C20" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C21" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B22" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C22" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B23" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C23" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B24" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C24" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B25" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C25" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B26" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C26" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B27" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C27" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B28" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C28" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>302</v>
+      </c>
+      <c r="B29" t="s">
         <v>305</v>
       </c>
-      <c r="B29" t="s">
-        <v>308</v>
-      </c>
       <c r="C29" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B30" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C30" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B31" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C31" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B32" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C32" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B33" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C33" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B34" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C34" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B35" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C35" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B36" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C36" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B37" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C37" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B38" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C38" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B39" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C39" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B40" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C40" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B41" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C41" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B42" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C42" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B43" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C43" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B44" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C44" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B45" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C45" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B46" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C46" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B47" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C47" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B48" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C48" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B49" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C49" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>341</v>
+      </c>
+      <c r="B50" t="s">
         <v>344</v>
       </c>
-      <c r="B50" t="s">
-        <v>347</v>
-      </c>
       <c r="C50" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B51" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C51" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B52" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C52" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>348</v>
+      </c>
+      <c r="B53" t="s">
         <v>351</v>
       </c>
-      <c r="B53" t="s">
-        <v>354</v>
-      </c>
       <c r="C53" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B54" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C54" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B55" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C55" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B56" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C56" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B57" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C57" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B58" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C58" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B59" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C59" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B60" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C60" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>365</v>
+      </c>
+      <c r="B61" t="s">
         <v>368</v>
       </c>
-      <c r="B61" t="s">
-        <v>371</v>
-      </c>
       <c r="C61" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B62" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C62" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>370</v>
+      </c>
+      <c r="B63" t="s">
+        <v>372</v>
+      </c>
+      <c r="C63" t="s">
         <v>373</v>
-      </c>
-      <c r="B63" t="s">
-        <v>375</v>
-      </c>
-      <c r="C63" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B64" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C64" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B65" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C65" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B66" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C66" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B67" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C67" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B68" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C68" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B69" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C69" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B70" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C70" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B71" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C71" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>388</v>
+      </c>
+      <c r="B72" t="s">
         <v>391</v>
       </c>
-      <c r="B72" t="s">
-        <v>394</v>
-      </c>
       <c r="C72" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B73" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C73" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B74" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C74" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B75" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C75" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>395</v>
+      </c>
+      <c r="B76" t="s">
         <v>398</v>
       </c>
-      <c r="B76" t="s">
-        <v>401</v>
-      </c>
       <c r="C76" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B77" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C77" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B78" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C78" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B79" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C79" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>403</v>
+      </c>
+      <c r="B80" t="s">
         <v>406</v>
       </c>
-      <c r="B80" t="s">
-        <v>409</v>
-      </c>
       <c r="C80" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B81" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C81" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B82" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C82" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>410</v>
+      </c>
+      <c r="B83" t="s">
         <v>413</v>
       </c>
-      <c r="B83" t="s">
-        <v>416</v>
-      </c>
       <c r="C83" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B84" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C84" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B85" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C85" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B86" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C86" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B87" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C87" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B88" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C88" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B89" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C89" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B90" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C90" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B91" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C91" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B92" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C92" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B93" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C93" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B94" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C94" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B95" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C95" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B96" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C96" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B97" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C97" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C98" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B99" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C99" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B100" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C100" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Farm History Survey 'psa_farm_history_survey' to V1.3
edited question 38 - added answer 38a. Updated all answer fields from integer to decimal
added note to question 43
</commit_message>
<xml_diff>
--- a/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
+++ b/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="460">
   <si>
     <t>type</t>
   </si>
@@ -1379,7 +1379,28 @@
     <t>Thank you for completing the Survey. The next screen has a timeline to share with your grower. Continue swiping until you reach the end to Submit.</t>
   </si>
   <si>
-    <t>v1.2</t>
+    <t>v1.3</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>I want to answer in $/ acre</t>
+  </si>
+  <si>
+    <t>econ_price_per_acre</t>
+  </si>
+  <si>
+    <t>38 a. Price per acre</t>
+  </si>
+  <si>
+    <t>Can answer on a field basis or per acre basis, but please indicate how you are answering</t>
+  </si>
+  <si>
+    <t>price_per_farm_acre</t>
+  </si>
+  <si>
+    <t>${econ} = 'price_per_farm_acre'</t>
   </si>
 </sst>
 </file>
@@ -1721,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2868,30 +2889,30 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>453</v>
       </c>
       <c r="B78" t="s">
-        <v>191</v>
+        <v>455</v>
       </c>
       <c r="C78" t="s">
-        <v>192</v>
-      </c>
-      <c r="E78" t="s">
-        <v>15</v>
+        <v>456</v>
+      </c>
+      <c r="E78" t="b">
+        <v>0</v>
       </c>
       <c r="H78" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>67</v>
+        <v>453</v>
       </c>
       <c r="B79" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C79" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E79" t="s">
         <v>15</v>
@@ -2902,30 +2923,30 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>67</v>
+        <v>453</v>
       </c>
       <c r="B80" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C80" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E80" t="s">
         <v>15</v>
       </c>
       <c r="H80" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>67</v>
+        <v>453</v>
       </c>
       <c r="B81" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C81" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -2936,13 +2957,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>453</v>
       </c>
       <c r="B82" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C82" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -2953,70 +2974,70 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>453</v>
       </c>
       <c r="B83" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C83" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
       </c>
       <c r="H83" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>67</v>
+        <v>453</v>
       </c>
       <c r="B84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C84" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
       </c>
       <c r="H84" t="s">
-        <v>205</v>
+        <v>459</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>45</v>
+        <v>453</v>
       </c>
       <c r="B85" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C85" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
       </c>
       <c r="H85" t="s">
-        <v>210</v>
+        <v>459</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B86" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C86" t="s">
-        <v>212</v>
-      </c>
-      <c r="D86" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
+      </c>
+      <c r="H86" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
@@ -3024,10 +3045,13 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C87" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="D87" t="s">
+        <v>213</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -3035,44 +3059,44 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C88" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
-      </c>
-      <c r="H88" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>219</v>
+        <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C89" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
+      </c>
+      <c r="H89" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B90" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -3080,13 +3104,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>45</v>
+        <v>222</v>
       </c>
       <c r="B91" t="s">
-        <v>444</v>
+        <v>223</v>
       </c>
       <c r="C91" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -3094,16 +3118,16 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>226</v>
+        <v>45</v>
       </c>
       <c r="B92" t="s">
-        <v>227</v>
+        <v>444</v>
       </c>
       <c r="C92" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D92" t="s">
-        <v>229</v>
+        <v>457</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -3111,13 +3135,16 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>45</v>
+        <v>226</v>
       </c>
       <c r="B93" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C93" t="s">
-        <v>231</v>
+        <v>228</v>
+      </c>
+      <c r="D93" t="s">
+        <v>229</v>
       </c>
       <c r="E93" t="s">
         <v>15</v>
@@ -3128,10 +3155,10 @@
         <v>45</v>
       </c>
       <c r="B94" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C94" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E94" t="s">
         <v>15</v>
@@ -3139,61 +3166,61 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B95" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C95" t="s">
-        <v>235</v>
-      </c>
-      <c r="D95" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E95" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C96" t="s">
-        <v>238</v>
+        <v>235</v>
+      </c>
+      <c r="D96" t="s">
+        <v>236</v>
       </c>
       <c r="E96" t="s">
         <v>48</v>
       </c>
-      <c r="H96" t="s">
-        <v>239</v>
-      </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>173</v>
+        <v>45</v>
       </c>
       <c r="B97" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C97" t="s">
-        <v>445</v>
+        <v>238</v>
       </c>
       <c r="E97" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="H97" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="B98" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C98" t="s">
-        <v>242</v>
+        <v>445</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -3201,13 +3228,13 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B99" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C99" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E99" t="s">
         <v>15</v>
@@ -3215,21 +3242,21 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>245</v>
+        <v>17</v>
+      </c>
+      <c r="B100" t="s">
+        <v>243</v>
+      </c>
+      <c r="C100" t="s">
+        <v>244</v>
+      </c>
+      <c r="E100" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>17</v>
-      </c>
-      <c r="B101" t="s">
-        <v>246</v>
-      </c>
-      <c r="C101" t="s">
-        <v>451</v>
-      </c>
-      <c r="E101" t="s">
-        <v>15</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
@@ -3237,16 +3264,13 @@
         <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C102" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="E102" t="s">
         <v>15</v>
-      </c>
-      <c r="K102" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
@@ -3254,26 +3278,43 @@
         <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C103" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
+      </c>
+      <c r="K103" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" t="s">
+        <v>248</v>
+      </c>
+      <c r="C104" t="s">
+        <v>450</v>
+      </c>
+      <c r="E104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>45</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>443</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>249</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E105" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3284,11 +3325,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -4109,10 +4155,10 @@
         <v>395</v>
       </c>
       <c r="B75" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="C75" t="s">
-        <v>397</v>
+        <v>454</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -4120,10 +4166,10 @@
         <v>395</v>
       </c>
       <c r="B76" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C76" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -4131,10 +4177,10 @@
         <v>395</v>
       </c>
       <c r="B77" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C77" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -4142,21 +4188,21 @@
         <v>395</v>
       </c>
       <c r="B78" t="s">
-        <v>402</v>
+        <v>458</v>
       </c>
       <c r="C78" t="s">
-        <v>297</v>
+        <v>401</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B79" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C79" t="s">
-        <v>405</v>
+        <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -4164,10 +4210,10 @@
         <v>403</v>
       </c>
       <c r="B80" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C80" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -4175,21 +4221,21 @@
         <v>403</v>
       </c>
       <c r="B81" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C81" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B82" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C82" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -4197,10 +4243,10 @@
         <v>410</v>
       </c>
       <c r="B83" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C83" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -4208,10 +4254,10 @@
         <v>410</v>
       </c>
       <c r="B84" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C84" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -4219,10 +4265,10 @@
         <v>410</v>
       </c>
       <c r="B85" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C85" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -4230,10 +4276,10 @@
         <v>410</v>
       </c>
       <c r="B86" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C86" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -4241,10 +4287,10 @@
         <v>410</v>
       </c>
       <c r="B87" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C87" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -4252,10 +4298,10 @@
         <v>410</v>
       </c>
       <c r="B88" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C88" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -4263,10 +4309,10 @@
         <v>410</v>
       </c>
       <c r="B89" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C89" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -4274,10 +4320,10 @@
         <v>410</v>
       </c>
       <c r="B90" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C90" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -4285,10 +4331,10 @@
         <v>410</v>
       </c>
       <c r="B91" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C91" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -4296,10 +4342,10 @@
         <v>410</v>
       </c>
       <c r="B92" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C92" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -4307,10 +4353,10 @@
         <v>410</v>
       </c>
       <c r="B93" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C93" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -4318,10 +4364,10 @@
         <v>410</v>
       </c>
       <c r="B94" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C94" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -4329,10 +4375,10 @@
         <v>410</v>
       </c>
       <c r="B95" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C95" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -4340,10 +4386,10 @@
         <v>410</v>
       </c>
       <c r="B96" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C96" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -4351,21 +4397,21 @@
         <v>410</v>
       </c>
       <c r="B97" t="s">
-        <v>296</v>
+        <v>439</v>
       </c>
       <c r="C97" t="s">
-        <v>297</v>
+        <v>440</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>441</v>
+        <v>410</v>
       </c>
       <c r="B98" t="s">
-        <v>262</v>
+        <v>296</v>
       </c>
       <c r="C98" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -4373,10 +4419,10 @@
         <v>441</v>
       </c>
       <c r="B99" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C99" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -4384,9 +4430,20 @@
         <v>441</v>
       </c>
       <c r="B100" t="s">
+        <v>266</v>
+      </c>
+      <c r="C100" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>441</v>
+      </c>
+      <c r="B101" t="s">
         <v>272</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>273</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add producer ID to psa_farm_history_survey
added producer ID
</commit_message>
<xml_diff>
--- a/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
+++ b/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="465">
   <si>
     <t>type</t>
   </si>
@@ -230,108 +230,66 @@
     <t>crop_acres</t>
   </si>
   <si>
-    <t>8. As of today, how many total acres do you plant in crops? [acres]</t>
-  </si>
-  <si>
     <t>select_multiple dq65c45</t>
   </si>
   <si>
     <t>farm_crop_rotation</t>
   </si>
   <si>
-    <t>9. What crops are GENERALLY in your crop rotation?</t>
-  </si>
-  <si>
     <t>cover_crop_acres</t>
   </si>
   <si>
-    <t>10. As of today, how many of your total cropped acres are in COVER CROPS? [acres]</t>
-  </si>
-  <si>
     <t>cover_crop_acres_terminated</t>
   </si>
   <si>
-    <t>10.a Clarification:  If COVER CROPS have already been terminated, how many acres did you have of winter cover crops prior to termination? [# acres, or leave blank if not applicable]</t>
-  </si>
-  <si>
     <t>${cover_crop_acres} = 0</t>
   </si>
   <si>
     <t>cover_crop_acres_typical</t>
   </si>
   <si>
-    <t>11.  If this was a particularly bad or otherwise non-representative year, how many acres do you typically have of winter COVER CROPS?  [# acres, or leave blank if not applicable]</t>
-  </si>
-  <si>
     <t>first_year_cover_crop</t>
   </si>
   <si>
-    <t>12. In what year did you first plant COVER CROPS? [four digit year, example : 1985] *reminder, for a grower to participate, this may not be their first time planting cover crops</t>
-  </si>
-  <si>
     <t>select_one xe2wp37</t>
   </si>
   <si>
     <t>every_year</t>
   </si>
   <si>
-    <t>13. Have you planted COVER CROPS every consecutive year since?</t>
-  </si>
-  <si>
     <t>cover_crop_rotation</t>
   </si>
   <si>
-    <t>13 a. If no, describe your cover crop rotation.</t>
-  </si>
-  <si>
     <t>select_one ny01y01</t>
   </si>
   <si>
     <t>favorite_cover_crop</t>
   </si>
   <si>
-    <t>14. Do you have a favorite cover crop?</t>
-  </si>
-  <si>
     <t>select_one xv1mj93</t>
   </si>
   <si>
     <t>favorite_winter_cover_crop</t>
   </si>
   <si>
-    <t>14a. Which is your favorite? (winter cover crop)</t>
-  </si>
-  <si>
     <t>${favorite_cover_crop} = 'yes'</t>
   </si>
   <si>
     <t>insured_acres</t>
   </si>
   <si>
-    <t>15. As of today, how many of your total cropped acres are enrolled in crop insurance? [acres]</t>
-  </si>
-  <si>
     <t>removed_insurance</t>
   </si>
   <si>
-    <t>16. Have you removed crop insurance on any of your fields due to cover cropping?</t>
-  </si>
-  <si>
     <t>if_yes_remove_insurance_note</t>
   </si>
   <si>
-    <t>16.a  If you selected "Yes," please provide additional details.</t>
-  </si>
-  <si>
     <t>${removed_insurance} = 'yes'</t>
   </si>
   <si>
     <t>claim_cover_crop</t>
   </si>
   <si>
-    <t>17.  Have you ever had problems filing a crop insurance claim because of using cover crops?</t>
-  </si>
-  <si>
     <t>if_yes_claim_note</t>
   </si>
   <si>
@@ -344,60 +302,39 @@
     <t>tilled_acres</t>
   </si>
   <si>
-    <t>18. As of today, how many of your total cropped acres are tilled? [# acres, enter "0" if none]</t>
-  </si>
-  <si>
     <t>select_one ow12s70</t>
   </si>
   <si>
     <t>farm_tillage_type</t>
   </si>
   <si>
-    <t>18.a Clarification:  Do you consider your operation:</t>
-  </si>
-  <si>
     <t>${tilled_acres} &gt; 0</t>
   </si>
   <si>
     <t>tillage_it_depends</t>
   </si>
   <si>
-    <t>18. a1 Clarification: If you selected "it depends", please describe.</t>
-  </si>
-  <si>
     <t>${farm_tillage_type} = 'depends'</t>
   </si>
   <si>
     <t>previous_tillage</t>
   </si>
   <si>
-    <t>18.b Clarification: Have you ever tilled any of your cropped acres?</t>
-  </si>
-  <si>
     <t>${tilled_acres} = 0</t>
   </si>
   <si>
     <t>years_since_tillage</t>
   </si>
   <si>
-    <t>18.c Clarification:  How many years since you last tilled any of your acres? [# of years]</t>
-  </si>
-  <si>
     <t>${previous_tillage} = 'yes' and ${tilled_acres} = 0</t>
   </si>
   <si>
     <t>tilled_acres_cover_crop</t>
   </si>
   <si>
-    <t>19. How many of your COVER CROPPED acres are tilled? [# of acres, enter "0" if none]</t>
-  </si>
-  <si>
     <t>tillage_type_cover_crop</t>
   </si>
   <si>
-    <t>19.a What kind of tillage are you doing on the COVER CROPPED acres?</t>
-  </si>
-  <si>
     <t>${tilled_acres_cover_crop} &gt; 0</t>
   </si>
   <si>
@@ -413,69 +350,39 @@
     <t>previous_tillage_cover_crop</t>
   </si>
   <si>
-    <t>19.b Clarification: Have you ever tilled your COVER CROPPED acres?</t>
-  </si>
-  <si>
     <t>${tilled_acres_cover_crop} = 0</t>
   </si>
   <si>
     <t>years_since_tillage_cover_crop</t>
   </si>
   <si>
-    <t>19.c Clarification: How many years since you last tilled your COVER CROPPED acres? [# of years]</t>
-  </si>
-  <si>
     <t>${previous_tillage_cover_crop} = 'yes' and ${tilled_acres_cover_crop} = 0</t>
   </si>
   <si>
     <t>info_sources</t>
   </si>
   <si>
-    <t>20. What sources of information do you seek out and use to learn more about cover crops?</t>
-  </si>
-  <si>
     <t>dst_use</t>
   </si>
   <si>
-    <t>21. Do you use any decision support tools. (e.g, spreadsheets, worksheets, or software tools provided by NRCS, extension specialists, or crop advisors)?</t>
-  </si>
-  <si>
     <t>software_use</t>
   </si>
   <si>
-    <t>22. What types of software, if any, do you use to manage your farm data?</t>
-  </si>
-  <si>
     <t>devices_use</t>
   </si>
   <si>
-    <t>23. What type of devices do you use in your agricultural operations (iPad, computer, smartphone)?</t>
-  </si>
-  <si>
     <t>yield_monitor</t>
   </si>
   <si>
-    <t>24. Where do you store your yield monitor data?</t>
-  </si>
-  <si>
     <t>yield_data_share</t>
   </si>
   <si>
-    <t>25. Do you feel comfortable sharing yield monitor data?</t>
-  </si>
-  <si>
     <t>percent_rented</t>
   </si>
   <si>
-    <t>26. Approximately what percentage of the acres you farm are rented?</t>
-  </si>
-  <si>
     <t>why_participating</t>
   </si>
   <si>
-    <t>27. Why are you participating in this study?</t>
-  </si>
-  <si>
     <t>generalfarmendnote</t>
   </si>
   <si>
@@ -509,57 +416,36 @@
     <t>years_cover_crop</t>
   </si>
   <si>
-    <t>28. How long has this site been cover cropped?</t>
-  </si>
-  <si>
     <t>insured</t>
   </si>
   <si>
-    <t>29. Is the trial field enrolled in crop insurance?</t>
-  </si>
-  <si>
     <t>select_one ab12c34</t>
   </si>
   <si>
     <t>rent_own</t>
   </si>
   <si>
-    <t>30. Is the trial field on rented or owned land?</t>
-  </si>
-  <si>
     <t>code_crop_rotation</t>
   </si>
   <si>
-    <t>31. What crops are GENERALLY in your crop rotation for this field?</t>
-  </si>
-  <si>
     <t>select_one dq65c45</t>
   </si>
   <si>
     <t>previous_crop</t>
   </si>
   <si>
-    <t>32. What was the previous crop last year in this field?</t>
-  </si>
-  <si>
     <t>select_multiple sv07f73</t>
   </si>
   <si>
     <t>previous_fert</t>
   </si>
   <si>
-    <t>33. How much total Nitrogen fertility was applied to the previous crop (approximately)? [lbs]</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
     <t>cover_crop_plant_date</t>
   </si>
   <si>
-    <t>34. When was the COVER CROP planted?</t>
-  </si>
-  <si>
     <t>If an exact date is not known, please enter approximately, to the closest week or month.</t>
   </si>
   <si>
@@ -569,33 +455,21 @@
     <t>cover_crop_planting_method</t>
   </si>
   <si>
-    <t>35. How was the cover crop planted?</t>
-  </si>
-  <si>
     <t>select_multiple xv1mj93</t>
   </si>
   <si>
     <t>cover_crop_spp</t>
   </si>
   <si>
-    <t>36. What cover crop species are planted?</t>
-  </si>
-  <si>
     <t>cover_crop_rate_total</t>
   </si>
   <si>
-    <t>37. What is the approximate total rate of all cover crop planted? (in lbs/ acre)</t>
-  </si>
-  <si>
     <t>select_one xs4gb03</t>
   </si>
   <si>
     <t>econ</t>
   </si>
   <si>
-    <t>38. How much do you pay for cover crop seed?</t>
-  </si>
-  <si>
     <t>econ_price_per_pound</t>
   </si>
   <si>
@@ -608,48 +482,30 @@
     <t>econ_price_seed_per_total_acres</t>
   </si>
   <si>
-    <t>38 c1. Price of seed for total cover crop acres</t>
-  </si>
-  <si>
     <t>${econ} = 'price_per_acre'</t>
   </si>
   <si>
     <t>econ_total_cover_acres</t>
   </si>
   <si>
-    <t>38 c2. Total cover crop acres</t>
-  </si>
-  <si>
     <t>econ_other</t>
   </si>
   <si>
-    <t>38 d. How much do you pay for cover crop seed: Other</t>
-  </si>
-  <si>
     <t>${econ} = 'price_other'</t>
   </si>
   <si>
     <t>cover_crop_litter</t>
   </si>
   <si>
-    <t>39. Do you apply litter, manure or fertility to your COVER CROP?</t>
-  </si>
-  <si>
     <t>Timeframe from cover crop planting to a month before crop planting.</t>
   </si>
   <si>
     <t>cover_crop_tillage</t>
   </si>
   <si>
-    <t>40. Do you do any tillage prior to terminating the COVER crop? (ie: subsoiling)</t>
-  </si>
-  <si>
     <t>cover_crop_tillage_type</t>
   </si>
   <si>
-    <t>40 a. If Yes, please describe?</t>
-  </si>
-  <si>
     <t>${cover_crop_tillage} = 'yes'</t>
   </si>
   <si>
@@ -659,9 +515,6 @@
     <t>cover_crop_termination</t>
   </si>
   <si>
-    <t>41. How do you terminate your COVER crop?</t>
-  </si>
-  <si>
     <t>select_multiple bd5he26</t>
   </si>
   <si>
@@ -701,9 +554,6 @@
     <t>more_farm_info</t>
   </si>
   <si>
-    <t>Are there other considerations or things you want us to know about this field? (why you plant cover crops there, it stays very wet, it's generally high biomass, it's new to cover crops, etc.)</t>
-  </si>
-  <si>
     <t>notegroupselect</t>
   </si>
   <si>
@@ -1325,9 +1175,6 @@
     <t>econ_price_per_acre</t>
   </si>
   <si>
-    <t>38 a. Price per acre</t>
-  </si>
-  <si>
     <t>Can answer on a field basis or per acre basis, but please indicate how you are answering</t>
   </si>
   <si>
@@ -1343,9 +1190,6 @@
     <t>Has this farmer participated previously? (If they have, you will skip the farmer interview portion and go directly to site history information.)</t>
   </si>
   <si>
-    <t>v2</t>
-  </si>
-  <si>
     <t>${farm_or_station} = 'farm' and ${previous_participant} = 'no'</t>
   </si>
   <si>
@@ -1376,37 +1220,202 @@
     <t>(If you plant green and use herbicide also, select "Herbicide". Planting Green will be asked next)</t>
   </si>
   <si>
-    <t>49. How much total Nitrogen fertilizer will this year's crop receive? (if you already selected that the COVER CROP received litter or manure, do not add it again here) (this can also include a combination of organic and inorganic fertility, please use an estimate of the combination)</t>
-  </si>
-  <si>
-    <t>48 a. If yes, please describe tillage.</t>
-  </si>
-  <si>
-    <t>48. Will you do any type of tillage on this crop?</t>
-  </si>
-  <si>
-    <t>47. What is the maturity of the crop? (ie, number of days to harvest or soybean maturity group, or other)</t>
-  </si>
-  <si>
-    <t>46. What is the variety of the crop?</t>
-  </si>
-  <si>
-    <t>45. What is/ will be this year's crop?</t>
-  </si>
-  <si>
-    <t>43. What herbicides do you plan to use?</t>
-  </si>
-  <si>
-    <t>42. Do you plant green?</t>
-  </si>
-  <si>
-    <t>44. How much money do you plan to spend on herbicides to terminate cover crops in this field ($0.00 / acre)</t>
-  </si>
-  <si>
-    <t>38 b1. Price per pound seed</t>
-  </si>
-  <si>
-    <t>38 b2. Pounds of seed per acre</t>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>8. Producer ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hint: Located on the Tech Dashboard &gt; Producer Information </t>
+  </si>
+  <si>
+    <t>producer_id</t>
+  </si>
+  <si>
+    <t>9. As of today, how many total acres do you plant in crops? [acres]</t>
+  </si>
+  <si>
+    <t>10. What crops are GENERALLY in your crop rotation?</t>
+  </si>
+  <si>
+    <t>111. As of today, how many of your total cropped acres are in COVER CROPS? [acres]</t>
+  </si>
+  <si>
+    <t>11.a Clarification:  If COVER CROPS have already been terminated, how many acres did you have of winter cover crops prior to termination? [# acres, or leave blank if not applicable]</t>
+  </si>
+  <si>
+    <t>12.  If this was a particularly bad or otherwise non-representative year, how many acres do you typically have of winter COVER CROPS?  [# acres, or leave blank if not applicable]</t>
+  </si>
+  <si>
+    <t>13. In what year did you first plant COVER CROPS? [four digit year, example : 1985] *reminder, for a grower to participate, this may not be their first time planting cover crops</t>
+  </si>
+  <si>
+    <t>14. Have you planted COVER CROPS every consecutive year since?</t>
+  </si>
+  <si>
+    <t>14 a. If no, describe your cover crop rotation.</t>
+  </si>
+  <si>
+    <t>15. Do you have a favorite cover crop?</t>
+  </si>
+  <si>
+    <t>15a. Which is your favorite? (winter cover crop)</t>
+  </si>
+  <si>
+    <t>16. As of today, how many of your total cropped acres are enrolled in crop insurance? [acres]</t>
+  </si>
+  <si>
+    <t>17. Have you removed crop insurance on any of your fields due to cover cropping?</t>
+  </si>
+  <si>
+    <t>18.  Have you ever had problems filing a crop insurance claim because of using cover crops?</t>
+  </si>
+  <si>
+    <t>18.a  If you selected "Yes," please provide additional details.</t>
+  </si>
+  <si>
+    <t>19. As of today, how many of your total cropped acres are tilled? [# acres, enter "0" if none]</t>
+  </si>
+  <si>
+    <t>19.a Clarification:  Do you consider your operation:</t>
+  </si>
+  <si>
+    <t>19.b Clarification: Have you ever tilled any of your cropped acres?</t>
+  </si>
+  <si>
+    <t>19.c Clarification:  How many years since you last tilled any of your acres? [# of years]</t>
+  </si>
+  <si>
+    <t>20. How many of your COVER CROPPED acres are tilled? [# of acres, enter "0" if none]</t>
+  </si>
+  <si>
+    <t>20.a What kind of tillage are you doing on the COVER CROPPED acres?</t>
+  </si>
+  <si>
+    <t>20. a1 Clarification: If you selected "it depends", please describe.</t>
+  </si>
+  <si>
+    <t>20.b Clarification: Have you ever tilled your COVER CROPPED acres?</t>
+  </si>
+  <si>
+    <t>20.c Clarification: How many years since you last tilled your COVER CROPPED acres? [# of years]</t>
+  </si>
+  <si>
+    <t>21. What sources of information do you seek out and use to learn more about cover crops?</t>
+  </si>
+  <si>
+    <t>22. Do you use any decision support tools. (e.g, spreadsheets, worksheets, or software tools provided by NRCS, extension specialists, or crop advisors)?</t>
+  </si>
+  <si>
+    <t>23. What types of software, if any, do you use to manage your farm data?</t>
+  </si>
+  <si>
+    <t>24. What type of devices do you use in your agricultural operations (iPad, computer, smartphone)?</t>
+  </si>
+  <si>
+    <t>25. Where do you store your yield monitor data?</t>
+  </si>
+  <si>
+    <t>26. Do you feel comfortable sharing yield monitor data?</t>
+  </si>
+  <si>
+    <t>27. Approximately what percentage of the acres you farm are rented?</t>
+  </si>
+  <si>
+    <t>28. Why are you participating in this study?</t>
+  </si>
+  <si>
+    <t>29. How long has this site been cover cropped?</t>
+  </si>
+  <si>
+    <t>30. Is the trial field enrolled in crop insurance?</t>
+  </si>
+  <si>
+    <t>31. Is the trial field on rented or owned land?</t>
+  </si>
+  <si>
+    <t>32. What crops are GENERALLY in your crop rotation for this field?</t>
+  </si>
+  <si>
+    <t>33. What was the previous crop last year in this field?</t>
+  </si>
+  <si>
+    <t>34. How much total Nitrogen fertility was applied to the previous crop (approximately)? [lbs]</t>
+  </si>
+  <si>
+    <t>35. When was the COVER CROP planted?</t>
+  </si>
+  <si>
+    <t>36. How was the cover crop planted?</t>
+  </si>
+  <si>
+    <t>37. What cover crop species are planted?</t>
+  </si>
+  <si>
+    <t>38. What is the approximate total rate of all cover crop planted? (in lbs/ acre)</t>
+  </si>
+  <si>
+    <t>39. How much do you pay for cover crop seed?</t>
+  </si>
+  <si>
+    <t>39 a. Price per acre</t>
+  </si>
+  <si>
+    <t>39 b1. Price per pound seed</t>
+  </si>
+  <si>
+    <t>39 b2. Pounds of seed per acre</t>
+  </si>
+  <si>
+    <t>39 c1. Price of seed for total cover crop acres</t>
+  </si>
+  <si>
+    <t>39 c2. Total cover crop acres</t>
+  </si>
+  <si>
+    <t>39 d. How much do you pay for cover crop seed: Other</t>
+  </si>
+  <si>
+    <t>40. Do you apply litter, manure or fertility to your COVER CROP?</t>
+  </si>
+  <si>
+    <t>41. Do you do any tillage prior to terminating the COVER crop? (ie: subsoiling)</t>
+  </si>
+  <si>
+    <t>41 a. If Yes, please describe?</t>
+  </si>
+  <si>
+    <t>42. How do you terminate your COVER crop?</t>
+  </si>
+  <si>
+    <t>43. Do you plant green?</t>
+  </si>
+  <si>
+    <t>44. What herbicides do you plan to use?</t>
+  </si>
+  <si>
+    <t>45. How much money do you plan to spend on herbicides to terminate cover crops in this field ($0.00 / acre)</t>
+  </si>
+  <si>
+    <t>46. What is/ will be this year's crop?</t>
+  </si>
+  <si>
+    <t>47. What is the variety of the crop?</t>
+  </si>
+  <si>
+    <t>48. What is the maturity of the crop? (ie, number of days to harvest or soybean maturity group, or other)</t>
+  </si>
+  <si>
+    <t>49. Will you do any type of tillage on this crop?</t>
+  </si>
+  <si>
+    <t>49 a. If yes, please describe tillage.</t>
+  </si>
+  <si>
+    <t>50. How much total Nitrogen fertilizer will this year's crop receive? (if you already selected that the COVER CROP received litter or manure, do not add it again here) (this can also include a combination of organic and inorganic fertility, please use an estimate of the combination)</t>
+  </si>
+  <si>
+    <t>51. Are there other considerations or things you want us to know about this field? (why you plant cover crops there, it stays very wet, it's generally high biomass, it's new to cover crops, etc.)</t>
   </si>
 </sst>
 </file>
@@ -1757,10 +1766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1799,10 +1808,10 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>425</v>
+        <v>375</v>
       </c>
       <c r="K1" t="s">
-        <v>426</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1860,7 +1869,7 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>422</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1877,7 +1886,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>440</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -2146,83 +2155,86 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>402</v>
+      </c>
+      <c r="C26" t="s">
+        <v>400</v>
+      </c>
+      <c r="D26" t="s">
+        <v>401</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>438</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>439</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>387</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" t="s">
-        <v>16</v>
+        <v>388</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>441</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>403</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
@@ -2230,13 +2242,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>404</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
@@ -2247,16 +2259,13 @@
         <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>405</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
-      </c>
-      <c r="H33" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2264,13 +2273,16 @@
         <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>406</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
+      </c>
+      <c r="H34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2278,10 +2290,10 @@
         <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>407</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -2289,13 +2301,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>408</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
@@ -2303,13 +2315,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>409</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
@@ -2317,13 +2329,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>410</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -2331,44 +2343,44 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>411</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
-      </c>
-      <c r="H39" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>412</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
+      </c>
+      <c r="H40" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>413</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -2376,132 +2388,129 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>414</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
-      </c>
-      <c r="H42" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" t="s">
         <v>87</v>
-      </c>
-      <c r="B43" t="s">
-        <v>101</v>
-      </c>
-      <c r="C43" t="s">
-        <v>102</v>
-      </c>
-      <c r="E43" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>415</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
-      </c>
-      <c r="H44" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>416</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
+      </c>
+      <c r="H45" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>417</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
-      </c>
-      <c r="H46" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>418</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C49" t="s">
-        <v>119</v>
+        <v>419</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -2509,95 +2518,98 @@
         <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
-        <v>122</v>
+        <v>420</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
+      </c>
+      <c r="H50" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>421</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
-      </c>
-      <c r="H51" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>422</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
       </c>
       <c r="H52" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>423</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
       </c>
       <c r="H53" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>424</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
       </c>
       <c r="H54" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>425</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
+      </c>
+      <c r="H55" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
@@ -2605,10 +2617,10 @@
         <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>426</v>
       </c>
       <c r="E56" t="s">
         <v>15</v>
@@ -2619,10 +2631,10 @@
         <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
+        <v>427</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
@@ -2633,10 +2645,10 @@
         <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="C58" t="s">
-        <v>142</v>
+        <v>428</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -2647,10 +2659,10 @@
         <v>45</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="C59" t="s">
-        <v>144</v>
+        <v>429</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2658,13 +2670,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B60" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>430</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2672,13 +2684,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="C61" t="s">
-        <v>148</v>
+        <v>431</v>
       </c>
       <c r="E61" t="s">
         <v>15</v>
@@ -2689,10 +2701,10 @@
         <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>150</v>
+        <v>432</v>
       </c>
       <c r="E62" t="s">
         <v>15</v>
@@ -2700,13 +2712,13 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="C63" t="s">
-        <v>152</v>
+        <v>433</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2714,77 +2726,77 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>120</v>
+      </c>
+      <c r="C64" t="s">
+        <v>121</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>153</v>
-      </c>
-      <c r="B65" t="s">
-        <v>154</v>
-      </c>
-      <c r="C65" t="s">
-        <v>155</v>
-      </c>
-      <c r="E65" t="s">
-        <v>15</v>
-      </c>
-      <c r="F65" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="C66" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
+      </c>
+      <c r="F66" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="C67" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="E67" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="B68" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C68" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="E68" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="C69" t="s">
-        <v>164</v>
+        <v>434</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -2792,13 +2804,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="C70" t="s">
-        <v>167</v>
+        <v>435</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2806,13 +2818,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="B71" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="C71" t="s">
-        <v>169</v>
+        <v>436</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2820,13 +2832,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>170</v>
+        <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="C72" t="s">
-        <v>172</v>
+        <v>437</v>
       </c>
       <c r="E72" t="s">
         <v>15</v>
@@ -2834,13 +2846,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="C73" t="s">
-        <v>175</v>
+        <v>438</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -2848,44 +2860,44 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>176</v>
+        <v>137</v>
       </c>
       <c r="B74" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
       <c r="C74" t="s">
-        <v>178</v>
-      </c>
-      <c r="D74" t="s">
-        <v>179</v>
-      </c>
-      <c r="E74" t="b">
-        <v>0</v>
+        <v>439</v>
+      </c>
+      <c r="E74" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="B75" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="C75" t="s">
-        <v>182</v>
-      </c>
-      <c r="E75" t="s">
-        <v>15</v>
+        <v>440</v>
+      </c>
+      <c r="D75" t="s">
+        <v>141</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="B76" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="C76" t="s">
-        <v>185</v>
+        <v>441</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
@@ -2893,13 +2905,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="B77" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="C77" t="s">
-        <v>187</v>
+        <v>442</v>
       </c>
       <c r="E77" t="s">
         <v>15</v>
@@ -2907,13 +2919,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="B78" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="C78" t="s">
-        <v>190</v>
+        <v>443</v>
       </c>
       <c r="E78" t="s">
         <v>15</v>
@@ -2921,132 +2933,132 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>431</v>
+        <v>147</v>
       </c>
       <c r="B79" t="s">
-        <v>433</v>
+        <v>148</v>
       </c>
       <c r="C79" t="s">
-        <v>434</v>
-      </c>
-      <c r="E79" t="b">
-        <v>0</v>
-      </c>
-      <c r="H79" t="s">
-        <v>196</v>
+        <v>444</v>
+      </c>
+      <c r="E79" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="B80" t="s">
-        <v>191</v>
+        <v>383</v>
       </c>
       <c r="C80" t="s">
-        <v>460</v>
-      </c>
-      <c r="E80" t="s">
-        <v>15</v>
+        <v>445</v>
+      </c>
+      <c r="E80" t="b">
+        <v>0</v>
       </c>
       <c r="H80" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="B81" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="C81" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
       </c>
       <c r="H81" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="B82" t="s">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="C82" t="s">
-        <v>195</v>
+        <v>447</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
       </c>
       <c r="H82" t="s">
-        <v>437</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="B83" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="C83" t="s">
-        <v>198</v>
+        <v>448</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
       </c>
       <c r="H83" t="s">
-        <v>437</v>
+        <v>386</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>45</v>
+        <v>381</v>
       </c>
       <c r="B84" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="C84" t="s">
-        <v>200</v>
+        <v>449</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
       </c>
       <c r="H84" t="s">
-        <v>201</v>
+        <v>386</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B85" t="s">
-        <v>202</v>
+        <v>155</v>
       </c>
       <c r="C85" t="s">
-        <v>203</v>
-      </c>
-      <c r="D85" t="s">
-        <v>204</v>
+        <v>450</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
+      </c>
+      <c r="H85" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B86" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="C86" t="s">
-        <v>206</v>
+        <v>451</v>
+      </c>
+      <c r="D86" t="s">
+        <v>158</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -3054,75 +3066,72 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B87" t="s">
-        <v>207</v>
+        <v>159</v>
       </c>
       <c r="C87" t="s">
-        <v>208</v>
+        <v>452</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
-      </c>
-      <c r="H87" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>210</v>
+        <v>45</v>
       </c>
       <c r="B88" t="s">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="C88" t="s">
-        <v>212</v>
-      </c>
-      <c r="D88" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
+      </c>
+      <c r="H88" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>445</v>
+        <v>162</v>
       </c>
       <c r="B89" t="s">
-        <v>446</v>
+        <v>163</v>
       </c>
       <c r="C89" t="s">
-        <v>458</v>
+        <v>454</v>
+      </c>
+      <c r="D89" t="s">
+        <v>398</v>
+      </c>
+      <c r="E89" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>213</v>
+        <v>393</v>
       </c>
       <c r="B90" t="s">
-        <v>214</v>
+        <v>394</v>
       </c>
       <c r="C90" t="s">
-        <v>457</v>
-      </c>
-      <c r="E90" t="s">
-        <v>15</v>
+        <v>455</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>431</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>424</v>
+        <v>165</v>
       </c>
       <c r="C91" t="s">
-        <v>459</v>
-      </c>
-      <c r="D91" t="s">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -3130,16 +3139,16 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>215</v>
+        <v>381</v>
       </c>
       <c r="B92" t="s">
-        <v>216</v>
+        <v>374</v>
       </c>
       <c r="C92" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D92" t="s">
-        <v>217</v>
+        <v>384</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -3147,13 +3156,16 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="B93" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
       <c r="C93" t="s">
-        <v>455</v>
+        <v>458</v>
+      </c>
+      <c r="D93" t="s">
+        <v>168</v>
       </c>
       <c r="E93" t="s">
         <v>15</v>
@@ -3164,10 +3176,10 @@
         <v>45</v>
       </c>
       <c r="B94" t="s">
-        <v>219</v>
+        <v>169</v>
       </c>
       <c r="C94" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="E94" t="s">
         <v>15</v>
@@ -3175,61 +3187,61 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B95" t="s">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="C95" t="s">
-        <v>453</v>
-      </c>
-      <c r="D95" t="s">
-        <v>221</v>
+        <v>460</v>
       </c>
       <c r="E95" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B96" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
       <c r="C96" t="s">
-        <v>452</v>
+        <v>461</v>
+      </c>
+      <c r="D96" t="s">
+        <v>172</v>
       </c>
       <c r="E96" t="s">
         <v>48</v>
       </c>
-      <c r="H96" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>45</v>
+      </c>
+      <c r="B97" t="s">
         <v>173</v>
       </c>
-      <c r="B97" t="s">
-        <v>224</v>
-      </c>
       <c r="C97" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="E97" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="H97" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="B98" t="s">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="C98" t="s">
-        <v>226</v>
+        <v>463</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -3237,13 +3249,13 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B99" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
       <c r="C99" t="s">
-        <v>228</v>
+        <v>464</v>
       </c>
       <c r="E99" t="s">
         <v>15</v>
@@ -3251,21 +3263,21 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>229</v>
+        <v>17</v>
+      </c>
+      <c r="B100" t="s">
+        <v>177</v>
+      </c>
+      <c r="C100" t="s">
+        <v>178</v>
+      </c>
+      <c r="E100" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>17</v>
-      </c>
-      <c r="B101" t="s">
-        <v>230</v>
-      </c>
-      <c r="C101" t="s">
-        <v>430</v>
-      </c>
-      <c r="E101" t="s">
-        <v>15</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
@@ -3273,16 +3285,13 @@
         <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>231</v>
+        <v>180</v>
       </c>
       <c r="C102" t="s">
-        <v>428</v>
+        <v>380</v>
       </c>
       <c r="E102" t="s">
         <v>15</v>
-      </c>
-      <c r="K102" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
@@ -3290,26 +3299,43 @@
         <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>232</v>
+        <v>181</v>
       </c>
       <c r="C103" t="s">
-        <v>429</v>
+        <v>378</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
+      </c>
+      <c r="K103" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" t="s">
+        <v>182</v>
+      </c>
+      <c r="C104" t="s">
+        <v>379</v>
+      </c>
+      <c r="E104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>45</v>
       </c>
-      <c r="B104" t="s">
-        <v>423</v>
-      </c>
-      <c r="C104" t="s">
-        <v>233</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="B105" t="s">
+        <v>373</v>
+      </c>
+      <c r="C105" t="s">
+        <v>183</v>
+      </c>
+      <c r="E105" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3335,7 +3361,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3346,1124 +3372,1124 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>241</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>242</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>244</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>247</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>249</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="C8" t="s">
-        <v>251</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s">
-        <v>253</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
-        <v>254</v>
+        <v>204</v>
       </c>
       <c r="C10" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>206</v>
       </c>
       <c r="C11" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
-        <v>259</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="C13" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="C14" t="s">
-        <v>263</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="C15" t="s">
-        <v>265</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
-        <v>267</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>268</v>
+        <v>218</v>
       </c>
       <c r="C17" t="s">
-        <v>269</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B18" t="s">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="C18" t="s">
-        <v>271</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B19" t="s">
-        <v>272</v>
+        <v>222</v>
       </c>
       <c r="C19" t="s">
-        <v>273</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s">
-        <v>274</v>
+        <v>224</v>
       </c>
       <c r="C20" t="s">
-        <v>275</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B21" t="s">
-        <v>276</v>
+        <v>226</v>
       </c>
       <c r="C21" t="s">
-        <v>277</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
       <c r="C22" t="s">
-        <v>279</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="C23" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>282</v>
+        <v>232</v>
       </c>
       <c r="B24" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="C24" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>282</v>
+        <v>232</v>
       </c>
       <c r="B25" t="s">
-        <v>284</v>
+        <v>234</v>
       </c>
       <c r="C25" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>285</v>
+        <v>235</v>
       </c>
       <c r="B26" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="C26" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>285</v>
+        <v>235</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B28" t="s">
-        <v>287</v>
+        <v>237</v>
       </c>
       <c r="C28" t="s">
-        <v>288</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B29" t="s">
-        <v>289</v>
+        <v>239</v>
       </c>
       <c r="C29" t="s">
-        <v>290</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B30" t="s">
-        <v>291</v>
+        <v>241</v>
       </c>
       <c r="C30" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B31" t="s">
-        <v>293</v>
+        <v>243</v>
       </c>
       <c r="C31" t="s">
-        <v>294</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B32" t="s">
-        <v>295</v>
+        <v>245</v>
       </c>
       <c r="C32" t="s">
-        <v>296</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B33" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="C33" t="s">
-        <v>265</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s">
-        <v>297</v>
+        <v>247</v>
       </c>
       <c r="C34" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B35" t="s">
-        <v>299</v>
+        <v>249</v>
       </c>
       <c r="C35" t="s">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B36" t="s">
-        <v>301</v>
+        <v>251</v>
       </c>
       <c r="C36" t="s">
-        <v>302</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B37" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="C37" t="s">
-        <v>304</v>
+        <v>254</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B38" t="s">
-        <v>305</v>
+        <v>255</v>
       </c>
       <c r="C38" t="s">
-        <v>306</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B39" t="s">
-        <v>307</v>
+        <v>257</v>
       </c>
       <c r="C39" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B40" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
       <c r="C40" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B41" t="s">
-        <v>311</v>
+        <v>261</v>
       </c>
       <c r="C41" t="s">
-        <v>312</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B42" t="s">
-        <v>313</v>
+        <v>263</v>
       </c>
       <c r="C42" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B43" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="C43" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B44" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="C44" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B45" t="s">
-        <v>319</v>
+        <v>269</v>
       </c>
       <c r="C45" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B46" t="s">
-        <v>321</v>
+        <v>271</v>
       </c>
       <c r="C46" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
       <c r="C47" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B48" t="s">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="C48" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="B49" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="C49" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="B50" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="C50" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="B51" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="C51" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B52" t="s">
-        <v>333</v>
+        <v>283</v>
       </c>
       <c r="C52" t="s">
-        <v>334</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B53" t="s">
-        <v>335</v>
+        <v>285</v>
       </c>
       <c r="C53" t="s">
-        <v>336</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B54" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="C54" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B55" t="s">
-        <v>339</v>
+        <v>289</v>
       </c>
       <c r="C55" t="s">
-        <v>340</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B56" t="s">
-        <v>341</v>
+        <v>291</v>
       </c>
       <c r="C56" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B57" t="s">
-        <v>343</v>
+        <v>293</v>
       </c>
       <c r="C57" t="s">
-        <v>344</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B58" t="s">
-        <v>345</v>
+        <v>295</v>
       </c>
       <c r="C58" t="s">
-        <v>346</v>
+        <v>296</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B59" t="s">
-        <v>347</v>
+        <v>297</v>
       </c>
       <c r="C59" t="s">
-        <v>348</v>
+        <v>298</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
       <c r="B60" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="C60" t="s">
-        <v>351</v>
+        <v>301</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
       <c r="B61" t="s">
-        <v>352</v>
+        <v>302</v>
       </c>
       <c r="C61" t="s">
-        <v>353</v>
+        <v>303</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B62" t="s">
-        <v>355</v>
+        <v>305</v>
       </c>
       <c r="C62" t="s">
-        <v>355</v>
+        <v>305</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B63" t="s">
-        <v>356</v>
+        <v>306</v>
       </c>
       <c r="C63" t="s">
-        <v>357</v>
+        <v>307</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B64" t="s">
-        <v>358</v>
+        <v>308</v>
       </c>
       <c r="C64" t="s">
-        <v>359</v>
+        <v>309</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B65" t="s">
-        <v>360</v>
+        <v>310</v>
       </c>
       <c r="C65" t="s">
-        <v>361</v>
+        <v>311</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B66" t="s">
-        <v>362</v>
+        <v>312</v>
       </c>
       <c r="C66" t="s">
-        <v>363</v>
+        <v>313</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B67" t="s">
-        <v>364</v>
+        <v>314</v>
       </c>
       <c r="C67" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B68" t="s">
-        <v>366</v>
+        <v>316</v>
       </c>
       <c r="C68" t="s">
-        <v>367</v>
+        <v>317</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B69" t="s">
-        <v>368</v>
+        <v>318</v>
       </c>
       <c r="C69" t="s">
-        <v>369</v>
+        <v>319</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B70" t="s">
-        <v>370</v>
+        <v>320</v>
       </c>
       <c r="C70" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="B71" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="C71" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="B72" t="s">
-        <v>375</v>
+        <v>325</v>
       </c>
       <c r="C72" t="s">
-        <v>376</v>
+        <v>326</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="B73" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="C73" t="s">
-        <v>378</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="B74" t="s">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="C74" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="B75" t="s">
+        <v>332</v>
+      </c>
+      <c r="C75" t="s">
         <v>382</v>
-      </c>
-      <c r="C75" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="B76" t="s">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="C76" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="B77" t="s">
-        <v>436</v>
+        <v>385</v>
       </c>
       <c r="C77" t="s">
-        <v>383</v>
+        <v>333</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="B78" t="s">
-        <v>384</v>
+        <v>334</v>
       </c>
       <c r="C78" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>385</v>
+        <v>335</v>
       </c>
       <c r="B79" t="s">
-        <v>386</v>
+        <v>336</v>
       </c>
       <c r="C79" t="s">
-        <v>449</v>
+        <v>397</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>385</v>
+        <v>335</v>
       </c>
       <c r="B80" t="s">
-        <v>387</v>
+        <v>337</v>
       </c>
       <c r="C80" t="s">
-        <v>444</v>
+        <v>392</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>385</v>
+        <v>335</v>
       </c>
       <c r="B81" t="s">
-        <v>388</v>
+        <v>338</v>
       </c>
       <c r="C81" t="s">
-        <v>389</v>
+        <v>339</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B82" t="s">
-        <v>391</v>
+        <v>341</v>
       </c>
       <c r="C82" t="s">
-        <v>392</v>
+        <v>342</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B83" t="s">
-        <v>393</v>
+        <v>343</v>
       </c>
       <c r="C83" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B84" t="s">
-        <v>395</v>
+        <v>345</v>
       </c>
       <c r="C84" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B85" t="s">
-        <v>397</v>
+        <v>347</v>
       </c>
       <c r="C85" t="s">
-        <v>398</v>
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B86" t="s">
-        <v>399</v>
+        <v>349</v>
       </c>
       <c r="C86" t="s">
-        <v>400</v>
+        <v>350</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B87" t="s">
-        <v>401</v>
+        <v>351</v>
       </c>
       <c r="C87" t="s">
-        <v>402</v>
+        <v>352</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B88" t="s">
-        <v>403</v>
+        <v>353</v>
       </c>
       <c r="C88" t="s">
-        <v>404</v>
+        <v>354</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B89" t="s">
-        <v>405</v>
+        <v>355</v>
       </c>
       <c r="C89" t="s">
-        <v>406</v>
+        <v>356</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B90" t="s">
-        <v>407</v>
+        <v>357</v>
       </c>
       <c r="C90" t="s">
-        <v>408</v>
+        <v>358</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B91" t="s">
-        <v>409</v>
+        <v>359</v>
       </c>
       <c r="C91" t="s">
-        <v>410</v>
+        <v>360</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B92" t="s">
-        <v>411</v>
+        <v>361</v>
       </c>
       <c r="C92" t="s">
-        <v>412</v>
+        <v>362</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B93" t="s">
-        <v>413</v>
+        <v>363</v>
       </c>
       <c r="C93" t="s">
-        <v>414</v>
+        <v>364</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B94" t="s">
-        <v>415</v>
+        <v>365</v>
       </c>
       <c r="C94" t="s">
-        <v>416</v>
+        <v>366</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B95" t="s">
-        <v>417</v>
+        <v>367</v>
       </c>
       <c r="C95" t="s">
-        <v>418</v>
+        <v>368</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B96" t="s">
-        <v>419</v>
+        <v>369</v>
       </c>
       <c r="C96" t="s">
-        <v>420</v>
+        <v>370</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>340</v>
+      </c>
+      <c r="B97" t="s">
         <v>390</v>
       </c>
-      <c r="B97" t="s">
-        <v>442</v>
-      </c>
       <c r="C97" t="s">
-        <v>443</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B98" t="s">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="C98" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>421</v>
+        <v>371</v>
       </c>
       <c r="B99" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="C99" t="s">
-        <v>247</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>421</v>
+        <v>371</v>
       </c>
       <c r="B100" t="s">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="C100" t="s">
-        <v>251</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>421</v>
+        <v>371</v>
       </c>
       <c r="B101" t="s">
-        <v>256</v>
+        <v>206</v>
       </c>
       <c r="C101" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>447</v>
+        <v>395</v>
       </c>
       <c r="B102" t="s">
-        <v>446</v>
+        <v>394</v>
       </c>
       <c r="C102" t="s">
-        <v>448</v>
+        <v>396</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>447</v>
+        <v>395</v>
       </c>
       <c r="B103" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="C103" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to producer ID clarifying note
Tell users to add at least 1 of 3 of producer identifiers:
1. Grower Phone
2. Grower Email
3. Producer ID
</commit_message>
<xml_diff>
--- a/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
+++ b/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="467">
   <si>
     <t>type</t>
   </si>
@@ -1238,9 +1238,6 @@
     <t>10. What crops are GENERALLY in your crop rotation?</t>
   </si>
   <si>
-    <t>111. As of today, how many of your total cropped acres are in COVER CROPS? [acres]</t>
-  </si>
-  <si>
     <t>11.a Clarification:  If COVER CROPS have already been terminated, how many acres did you have of winter cover crops prior to termination? [# acres, or leave blank if not applicable]</t>
   </si>
   <si>
@@ -1416,6 +1413,15 @@
   </si>
   <si>
     <t>51. Are there other considerations or things you want us to know about this field? (why you plant cover crops there, it stays very wet, it's generally high biomass, it's new to cover crops, etc.)</t>
+  </si>
+  <si>
+    <t>producer_id_note</t>
+  </si>
+  <si>
+    <t>Enter at least 1 of 3 of the following producer identifiers</t>
+  </si>
+  <si>
+    <t>11. As of today, how many of your total cropped acres are in COVER CROPS? [acres]</t>
   </si>
 </sst>
 </file>
@@ -1766,10 +1772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2127,16 +2133,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>464</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" t="s">
-        <v>15</v>
+        <v>465</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2144,10 +2150,10 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -2158,97 +2164,97 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>402</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>400</v>
-      </c>
-      <c r="D26" t="s">
-        <v>401</v>
-      </c>
-      <c r="E26" t="b">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>402</v>
+      </c>
+      <c r="C27" t="s">
+        <v>400</v>
+      </c>
+      <c r="D27" t="s">
+        <v>401</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>387</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>388</v>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>387</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" t="s">
-        <v>16</v>
+        <v>388</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>389</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>403</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
@@ -2256,13 +2262,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -2273,16 +2279,13 @@
         <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>406</v>
+        <v>466</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
-      </c>
-      <c r="H34" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2290,13 +2293,16 @@
         <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2304,10 +2310,10 @@
         <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
@@ -2315,13 +2321,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
@@ -2329,13 +2335,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -2343,13 +2349,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -2357,44 +2363,44 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
-      </c>
-      <c r="H40" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
+      </c>
+      <c r="H41" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
@@ -2402,132 +2408,129 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>413</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
-      </c>
-      <c r="H43" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>415</v>
+        <v>90</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
+      </c>
+      <c r="H44" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
-      </c>
-      <c r="H45" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
+      </c>
+      <c r="H46" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
-      </c>
-      <c r="H47" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>417</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>419</v>
+        <v>106</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
       </c>
       <c r="H50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -2535,95 +2538,98 @@
         <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
+      </c>
+      <c r="H51" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
-      </c>
-      <c r="H52" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C53" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
       </c>
       <c r="H53" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C54" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
       </c>
       <c r="H54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
       </c>
       <c r="H55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C56" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E56" t="s">
         <v>15</v>
+      </c>
+      <c r="H56" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
@@ -2631,10 +2637,10 @@
         <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C57" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
@@ -2645,10 +2651,10 @@
         <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -2659,10 +2665,10 @@
         <v>45</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2673,10 +2679,10 @@
         <v>45</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C60" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2684,13 +2690,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C61" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E61" t="s">
         <v>15</v>
@@ -2698,13 +2704,13 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E62" t="s">
         <v>15</v>
@@ -2715,10 +2721,10 @@
         <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C63" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2726,240 +2732,237 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" t="s">
+        <v>432</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>17</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>120</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>121</v>
       </c>
-      <c r="E64" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>122</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>123</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>124</v>
       </c>
-      <c r="E66" t="s">
-        <v>15</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>17</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>125</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>126</v>
       </c>
-      <c r="E67" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+      <c r="E68" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>45</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>127</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>128</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E69" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>129</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>130</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
+        <v>433</v>
+      </c>
+      <c r="E70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" t="s">
         <v>434</v>
       </c>
-      <c r="E69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>76</v>
-      </c>
-      <c r="B70" t="s">
-        <v>131</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="E71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72" t="s">
         <v>435</v>
       </c>
-      <c r="E70" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>132</v>
-      </c>
-      <c r="B71" t="s">
-        <v>133</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="E72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" t="s">
         <v>436</v>
       </c>
-      <c r="E71" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" t="s">
-        <v>134</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>135</v>
+      </c>
+      <c r="B74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" t="s">
         <v>437</v>
       </c>
-      <c r="E72" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>135</v>
-      </c>
-      <c r="B73" t="s">
-        <v>136</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="E74" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" t="s">
         <v>438</v>
       </c>
-      <c r="E73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>137</v>
-      </c>
-      <c r="B74" t="s">
-        <v>138</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="E75" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" t="s">
         <v>439</v>
       </c>
-      <c r="E74" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>139</v>
-      </c>
-      <c r="B75" t="s">
-        <v>140</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="D76" t="s">
+        <v>141</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>142</v>
+      </c>
+      <c r="B77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C77" t="s">
         <v>440</v>
       </c>
-      <c r="D75" t="s">
-        <v>141</v>
-      </c>
-      <c r="E75" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>142</v>
-      </c>
-      <c r="B76" t="s">
-        <v>143</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="E77" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>144</v>
+      </c>
+      <c r="B78" t="s">
+        <v>145</v>
+      </c>
+      <c r="C78" t="s">
         <v>441</v>
       </c>
-      <c r="E76" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>144</v>
-      </c>
-      <c r="B77" t="s">
-        <v>145</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="E78" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" t="s">
         <v>442</v>
       </c>
-      <c r="E77" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>67</v>
-      </c>
-      <c r="B78" t="s">
-        <v>146</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="E79" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>147</v>
+      </c>
+      <c r="B80" t="s">
+        <v>148</v>
+      </c>
+      <c r="C80" t="s">
         <v>443</v>
       </c>
-      <c r="E78" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>147</v>
-      </c>
-      <c r="B79" t="s">
-        <v>148</v>
-      </c>
-      <c r="C79" t="s">
-        <v>444</v>
-      </c>
-      <c r="E79" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>381</v>
-      </c>
-      <c r="B80" t="s">
-        <v>383</v>
-      </c>
-      <c r="C80" t="s">
-        <v>445</v>
-      </c>
-      <c r="E80" t="b">
-        <v>0</v>
-      </c>
-      <c r="H80" t="s">
-        <v>153</v>
+      <c r="E80" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
@@ -2967,16 +2970,16 @@
         <v>381</v>
       </c>
       <c r="B81" t="s">
-        <v>149</v>
+        <v>383</v>
       </c>
       <c r="C81" t="s">
-        <v>446</v>
-      </c>
-      <c r="E81" t="s">
-        <v>15</v>
+        <v>444</v>
+      </c>
+      <c r="E81" t="b">
+        <v>0</v>
       </c>
       <c r="H81" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
@@ -2984,10 +2987,10 @@
         <v>381</v>
       </c>
       <c r="B82" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C82" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -3001,16 +3004,16 @@
         <v>381</v>
       </c>
       <c r="B83" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C83" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
       </c>
       <c r="H83" t="s">
-        <v>386</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
@@ -3018,10 +3021,10 @@
         <v>381</v>
       </c>
       <c r="B84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C84" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -3032,36 +3035,36 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>45</v>
+        <v>381</v>
       </c>
       <c r="B85" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C85" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
       </c>
       <c r="H85" t="s">
-        <v>156</v>
+        <v>386</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B86" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C86" t="s">
-        <v>451</v>
-      </c>
-      <c r="D86" t="s">
-        <v>158</v>
+        <v>449</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
+      </c>
+      <c r="H86" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
@@ -3069,10 +3072,13 @@
         <v>79</v>
       </c>
       <c r="B87" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C87" t="s">
-        <v>452</v>
+        <v>450</v>
+      </c>
+      <c r="D87" t="s">
+        <v>158</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -3080,75 +3086,72 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B88" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C88" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
-      </c>
-      <c r="H88" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>162</v>
+        <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C89" t="s">
-        <v>454</v>
-      </c>
-      <c r="D89" t="s">
-        <v>398</v>
+        <v>452</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
+      </c>
+      <c r="H89" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>393</v>
+        <v>162</v>
       </c>
       <c r="B90" t="s">
-        <v>394</v>
+        <v>163</v>
       </c>
       <c r="C90" t="s">
-        <v>455</v>
+        <v>453</v>
+      </c>
+      <c r="D90" t="s">
+        <v>398</v>
+      </c>
+      <c r="E90" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>164</v>
+        <v>393</v>
       </c>
       <c r="B91" t="s">
-        <v>165</v>
+        <v>394</v>
       </c>
       <c r="C91" t="s">
-        <v>456</v>
-      </c>
-      <c r="E91" t="s">
-        <v>15</v>
+        <v>454</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>381</v>
+        <v>164</v>
       </c>
       <c r="B92" t="s">
-        <v>374</v>
+        <v>165</v>
       </c>
       <c r="C92" t="s">
-        <v>457</v>
-      </c>
-      <c r="D92" t="s">
-        <v>384</v>
+        <v>455</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -3156,16 +3159,16 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>166</v>
+        <v>381</v>
       </c>
       <c r="B93" t="s">
-        <v>167</v>
+        <v>374</v>
       </c>
       <c r="C93" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D93" t="s">
-        <v>168</v>
+        <v>384</v>
       </c>
       <c r="E93" t="s">
         <v>15</v>
@@ -3173,13 +3176,16 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="B94" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C94" t="s">
-        <v>459</v>
+        <v>457</v>
+      </c>
+      <c r="D94" t="s">
+        <v>168</v>
       </c>
       <c r="E94" t="s">
         <v>15</v>
@@ -3190,10 +3196,10 @@
         <v>45</v>
       </c>
       <c r="B95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C95" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E95" t="s">
         <v>15</v>
@@ -3201,61 +3207,61 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B96" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C96" t="s">
-        <v>461</v>
-      </c>
-      <c r="D96" t="s">
-        <v>172</v>
+        <v>459</v>
       </c>
       <c r="E96" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B97" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C97" t="s">
-        <v>462</v>
+        <v>460</v>
+      </c>
+      <c r="D97" t="s">
+        <v>172</v>
       </c>
       <c r="E97" t="s">
         <v>48</v>
       </c>
-      <c r="H97" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="B98" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C98" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E98" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="H98" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="B99" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C99" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E99" t="s">
         <v>15</v>
@@ -3263,13 +3269,13 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B100" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C100" t="s">
-        <v>178</v>
+        <v>463</v>
       </c>
       <c r="E100" t="s">
         <v>15</v>
@@ -3277,21 +3283,21 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>179</v>
+        <v>17</v>
+      </c>
+      <c r="B101" t="s">
+        <v>177</v>
+      </c>
+      <c r="C101" t="s">
+        <v>178</v>
+      </c>
+      <c r="E101" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>17</v>
-      </c>
-      <c r="B102" t="s">
-        <v>180</v>
-      </c>
-      <c r="C102" t="s">
-        <v>380</v>
-      </c>
-      <c r="E102" t="s">
-        <v>15</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
@@ -3299,16 +3305,13 @@
         <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C103" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
-      </c>
-      <c r="K103" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.35">
@@ -3316,26 +3319,43 @@
         <v>17</v>
       </c>
       <c r="B104" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C104" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E104" t="s">
         <v>15</v>
+      </c>
+      <c r="K104" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>17</v>
+      </c>
+      <c r="B105" t="s">
+        <v>182</v>
+      </c>
+      <c r="C105" t="s">
+        <v>379</v>
+      </c>
+      <c r="E105" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>45</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>373</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>183</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E106" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
psa_farm _history updated cc_planting methods
Updated the choices in the cc_planting_methods . removed "other" added "natural_seeded"
</commit_message>
<xml_diff>
--- a/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
+++ b/forms/psa_farm_history_survey/psa_farm_history_survey.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="469">
   <si>
     <t>type</t>
   </si>
@@ -1422,6 +1422,12 @@
   </si>
   <si>
     <t>11. As of today, how many of your total cropped acres are in COVER CROPS? [acres]</t>
+  </si>
+  <si>
+    <t>Natural Seeded</t>
+  </si>
+  <si>
+    <t>natural_seeded</t>
   </si>
 </sst>
 </file>
@@ -1774,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3369,14 +3375,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="25.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -4187,10 +4193,10 @@
         <v>322</v>
       </c>
       <c r="B74" t="s">
-        <v>230</v>
+        <v>468</v>
       </c>
       <c r="C74" t="s">
-        <v>231</v>
+        <v>467</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>